<commit_message>
a new version of CA_Market dataset is created. bags and shirts attributes have been corrected
</commit_message>
<xml_diff>
--- a/results/mean_metrics_all.xlsx
+++ b/results/mean_metrics_all.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t xml:space="preserve">mb_12_nowei</t>
   </si>
@@ -57,7 +57,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -86,12 +86,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,7 +137,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -153,10 +147,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -177,10 +167,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -194,10 +184,10 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -285,6 +275,75 @@
         <v>0.564864754676819</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>0.5813</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>0.3277</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>0.5413</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>0.3934</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>0.328</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>0.5434</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>0.3816</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>0.311</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>0.71688574552536</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>0.634228229522705</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>0.602592468261719</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>